<commit_message>
Changed path of destination file as previous file was a test file. Confirmed that it worked after running.
</commit_message>
<xml_diff>
--- a/ExperianDailyAverage.xlsx
+++ b/ExperianDailyAverage.xlsx
@@ -39,12 +39,12 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">01/08/2022</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">02/08/2022</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">03/08/2022</t>
     </r>
   </si>
 </sst>
@@ -270,16 +270,16 @@
         <v>5</v>
       </c>
       <c r="B2" s="3">
-        <v>83.23</v>
+        <v>85.1</v>
       </c>
       <c r="C2" s="3">
-        <v>182.1</v>
+        <v>180.7</v>
       </c>
       <c r="D2" s="3">
-        <v>192.15</v>
+        <v>190.84</v>
       </c>
       <c r="E2" s="3">
-        <v>194.74</v>
+        <v>194.14</v>
       </c>
     </row>
     <row r="3" ht="16.560000" customHeight="1">
@@ -287,16 +287,16 @@
         <v>6</v>
       </c>
       <c r="B3" s="5">
-        <v>85.1</v>
+        <v>85.71</v>
       </c>
       <c r="C3" s="5">
-        <v>180.7</v>
+        <v>179.8</v>
       </c>
       <c r="D3" s="5">
-        <v>190.75</v>
+        <v>190.01</v>
       </c>
       <c r="E3" s="5">
-        <v>194.15</v>
+        <v>192.79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added email notification functionality that gives 3 different email outcomes.
</commit_message>
<xml_diff>
--- a/ExperianDailyAverage.xlsx
+++ b/ExperianDailyAverage.xlsx
@@ -39,12 +39,12 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">02/08/2022</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">03/08/2022</t>
+      <t xml:space="preserve">09/08/2022</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">10/08/2022</t>
     </r>
   </si>
 </sst>
@@ -270,16 +270,16 @@
         <v>5</v>
       </c>
       <c r="B2" s="3">
-        <v>85.1</v>
+        <v>88.59</v>
       </c>
       <c r="C2" s="3">
-        <v>180.7</v>
+        <v>175.77</v>
       </c>
       <c r="D2" s="3">
-        <v>190.84</v>
+        <v>186.41</v>
       </c>
       <c r="E2" s="3">
-        <v>194.14</v>
+        <v>189.47</v>
       </c>
     </row>
     <row r="3" ht="16.560000" customHeight="1">
@@ -287,16 +287,16 @@
         <v>6</v>
       </c>
       <c r="B3" s="5">
-        <v>85.71</v>
+        <v>85.77</v>
       </c>
       <c r="C3" s="5">
-        <v>179.8</v>
+        <v>175.24</v>
       </c>
       <c r="D3" s="5">
-        <v>190.01</v>
+        <v>185.9</v>
       </c>
       <c r="E3" s="5">
-        <v>192.79</v>
+        <v>188.42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>